<commit_message>
default title doesn't include file extension; lucene index has metadata and facetted metadata
</commit_message>
<xml_diff>
--- a/src/test/resources/org/voyanttools/trombone/texts/formats/chars.xlsx
+++ b/src/test/resources/org/voyanttools/trombone/texts/formats/chars.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Il était une fois</t>
-  </si>
-  <si>
     <t>Un &lt;texte&gt; intéressant &amp; un test.</t>
   </si>
   <si>
@@ -36,6 +33,9 @@
   </si>
   <si>
     <t>phrase 2</t>
+  </si>
+  <si>
+    <t>Il était une fois.</t>
   </si>
 </sst>
 </file>
@@ -360,18 +360,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>